<commit_message>
count characters in a string
</commit_message>
<xml_diff>
--- a/To_Do/to_do.xlsx
+++ b/To_Do/to_do.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI\Basic\python exercises\To_Do\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919B5EE7-7F89-4CA1-99F4-4135DB2B33DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73B0952-849F-48B7-8381-FE034C18B5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1176,7 +1176,7 @@
       <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="28.5">
       <c r="A14" s="2">

</xml_diff>